<commit_message>
update bomlist of pump monitoring system.
</commit_message>
<xml_diff>
--- a/project/PumpMonitoring/171020_PumpMonitoring/bomlist.xlsx
+++ b/project/PumpMonitoring/171020_PumpMonitoring/bomlist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="185">
   <si>
     <t>Part</t>
   </si>
@@ -691,6 +691,29 @@
     </rPh>
     <rPh sb="25" eb="26">
       <t>オナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C0603</t>
+  </si>
+  <si>
+    <t>(43.18 26.67)</t>
+  </si>
+  <si>
+    <t>NC</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>新規追加</t>
+    <rPh sb="0" eb="2">
+      <t>シンキ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ツイカ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -699,7 +722,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -721,6 +744,22 @@
       <color theme="10"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -825,7 +864,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -869,6 +908,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1173,10 +1218,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1275,93 +1320,95 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="A4" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="E4" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="I4" s="16"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A6" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D6" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14" t="s">
+      <c r="G6" s="14"/>
+      <c r="H6" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="I5" s="14"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="I6" s="1"/>
+      <c r="I6" s="14"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>26</v>
@@ -1376,20 +1423,20 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>159</v>
@@ -1401,20 +1448,20 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>159</v>
@@ -1426,17 +1473,17 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>26</v>
@@ -1449,80 +1496,76 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H11" s="2" t="s">
+      <c r="G12" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>160</v>
-      </c>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>159</v>
@@ -1530,67 +1573,69 @@
       <c r="H13" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I13" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A14" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="12" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>57</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>156</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>61</v>
@@ -1602,7 +1647,7 @@
         <v>57</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>64</v>
@@ -1617,7 +1662,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A17" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>61</v>
@@ -1629,10 +1674,10 @@
         <v>57</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>156</v>
@@ -1644,7 +1689,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>61</v>
@@ -1656,10 +1701,10 @@
         <v>57</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>156</v>
@@ -1671,19 +1716,19 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A19" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>57</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>20</v>
@@ -1693,68 +1738,66 @@
       </c>
       <c r="H19" s="11"/>
       <c r="I19" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A20" s="11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>57</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="G20" s="11" t="s">
         <v>156</v>
       </c>
       <c r="H20" s="11"/>
       <c r="I20" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A21" s="11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>57</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="H21" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>179</v>
+      <c r="H21" s="11"/>
+      <c r="I21" s="12" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>72</v>
@@ -1766,7 +1809,7 @@
         <v>57</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>59</v>
@@ -1782,31 +1825,37 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A23" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F23" s="1" t="s">
+      <c r="A23" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="G23" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
@@ -1816,7 +1865,7 @@
         <v>85</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>59</v>
@@ -1828,38 +1877,34 @@
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A25" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="F25" s="9" t="s">
+      <c r="A25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G25" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9" t="s">
-        <v>152</v>
-      </c>
+      <c r="G25" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="9" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>91</v>
@@ -1868,7 +1913,7 @@
         <v>92</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>59</v>
@@ -1883,10 +1928,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>91</v>
@@ -1895,7 +1940,7 @@
         <v>92</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>59</v>
@@ -1910,7 +1955,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>90</v>
@@ -1922,7 +1967,7 @@
         <v>92</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>59</v>
@@ -1937,7 +1982,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A29" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>90</v>
@@ -1949,7 +1994,7 @@
         <v>92</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>59</v>
@@ -1963,33 +2008,35 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A30" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
+      <c r="A30" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>104</v>
@@ -2001,10 +2048,10 @@
         <v>106</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>159</v>
@@ -2014,7 +2061,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>104</v>
@@ -2026,7 +2073,7 @@
         <v>106</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>78</v>
@@ -2039,7 +2086,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>104</v>
@@ -2051,7 +2098,7 @@
         <v>106</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>78</v>
@@ -2064,7 +2111,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>104</v>
@@ -2076,7 +2123,7 @@
         <v>106</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>78</v>
@@ -2087,64 +2134,64 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="27" x14ac:dyDescent="0.15">
-      <c r="A35" s="11" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A35" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+      <c r="A36" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="B35" s="11">
+      <c r="B36" s="11">
         <v>10</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C36" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D36" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E36" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F36" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="G35" s="13" t="s">
+      <c r="G36" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="H35" s="13"/>
-      <c r="I35" s="12" t="s">
+      <c r="H36" s="13"/>
+      <c r="I36" s="12" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A36" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>105</v>
@@ -2153,21 +2200,23 @@
         <v>106</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G37" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>105</v>
@@ -2176,20 +2225,18 @@
         <v>106</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>159</v>
-      </c>
+      <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>104</v>
@@ -2201,7 +2248,7 @@
         <v>106</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>78</v>
@@ -2214,10 +2261,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>105</v>
@@ -2226,7 +2273,7 @@
         <v>106</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>78</v>
@@ -2239,7 +2286,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>129</v>
@@ -2251,166 +2298,164 @@
         <v>106</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>78</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>52</v>
+        <v>106</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="H42" s="1"/>
-      <c r="I42" s="3" t="s">
-        <v>174</v>
-      </c>
+      <c r="I42" s="1"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>138</v>
+        <v>52</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>159</v>
       </c>
       <c r="H43" s="1"/>
-      <c r="I43" s="1" t="s">
-        <v>158</v>
+      <c r="I43" s="3" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>159</v>
       </c>
       <c r="H44" s="1"/>
-      <c r="I44" s="3" t="s">
-        <v>175</v>
+      <c r="I44" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H45" s="1"/>
+      <c r="I45" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A46" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-    </row>
-    <row r="46" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.15"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+    </row>
     <row r="47" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A48" s="4" t="s">
+    <row r="48" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A49" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A49" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1" t="s">
-        <v>152</v>
-      </c>
+      <c r="B49" s="7"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>168</v>
@@ -2422,10 +2467,10 @@
         <v>170</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>159</v>
@@ -2435,20 +2480,47 @@
         <v>152</v>
       </c>
     </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A51" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <hyperlinks>
-    <hyperlink ref="I44" r:id="rId1"/>
-    <hyperlink ref="I42" r:id="rId2"/>
-    <hyperlink ref="I15" r:id="rId3"/>
-    <hyperlink ref="I16" r:id="rId4"/>
-    <hyperlink ref="I17" r:id="rId5"/>
-    <hyperlink ref="I18" r:id="rId6"/>
-    <hyperlink ref="I19" r:id="rId7"/>
-    <hyperlink ref="I14" r:id="rId8"/>
-    <hyperlink ref="I20" r:id="rId9"/>
-    <hyperlink ref="I35" r:id="rId10"/>
-    <hyperlink ref="I12" r:id="rId11"/>
+    <hyperlink ref="I45" r:id="rId1"/>
+    <hyperlink ref="I43" r:id="rId2"/>
+    <hyperlink ref="I16" r:id="rId3"/>
+    <hyperlink ref="I17" r:id="rId4"/>
+    <hyperlink ref="I18" r:id="rId5"/>
+    <hyperlink ref="I19" r:id="rId6"/>
+    <hyperlink ref="I20" r:id="rId7"/>
+    <hyperlink ref="I15" r:id="rId8"/>
+    <hyperlink ref="I21" r:id="rId9"/>
+    <hyperlink ref="I36" r:id="rId10"/>
+    <hyperlink ref="I13" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>

</xml_diff>